<commit_message>
fix: a few bugs related to old versions of packages. More robust handling of default data sheet specification
</commit_message>
<xml_diff>
--- a/templates/default-template.xlsx
+++ b/templates/default-template.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jscott4\OneDrive - Department for Education\Documents\quickReport\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jscott4\OneDrive - Department for Education\Documents\quickReport1\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C4890F-9841-45B6-B831-87ED76A4C06C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB5DB70-F716-436A-AB4A-9453E567B77B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8446EDBA-5D18-4799-B725-1451DE8DD060}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8446EDBA-5D18-4799-B725-1451DE8DD060}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Data Sheets" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,12 +35,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Data exported using R package {quickReport}</t>
   </si>
   <si>
     <t>Report Information</t>
+  </si>
+  <si>
+    <t>!data</t>
   </si>
 </sst>
 </file>
@@ -416,7 +420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFD4D8D-F48B-49D7-B571-2E78D7B5C855}">
   <dimension ref="B2:L38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
@@ -494,4 +498,24 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8ABCC59-F944-4E6A-928F-F9EFEE2EA45D}">
+  <dimension ref="B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>